<commit_message>
made progress on excell files
</commit_message>
<xml_diff>
--- a/data/Food_nutrition_Intake/food_table1.xlsx
+++ b/data/Food_nutrition_Intake/food_table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20201077\Desktop\DorukGüngör\Eindhoven\Data_Science_AI\Knowledge_Engineering\Knowledge-Engineering-2AMD20-\data\Food_nutrition_Intake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B05961-ABD6-44C7-B1AA-F29E36F1248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C253B71-FA79-42E4-9340-9AD066EF844C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,24 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="42">
   <si>
     <t>Food group</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   Total population</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">      Household income &lt; 185% poverty line</t>
@@ -88,21 +73,6 @@
     <t>Vegetables: red and orange without tomatoes (cup)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">      Seniors age 65 and above</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">      Children age 2–19</t>
   </si>
   <si>
@@ -148,21 +118,6 @@
         <family val="2"/>
       </rPr>
       <t>School foods eaten by those age 20 and above are classified as other food away from home.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      Adults age 20–64</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
     </r>
   </si>
   <si>
@@ -234,6 +189,18 @@
   </si>
   <si>
     <t>Other 2017 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Total population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Adults age 20–64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Seniors age 65 and above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Adults age 20–6</t>
   </si>
 </sst>
 </file>
@@ -1385,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,51 +1377,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="22" t="s">
+      <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="N1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1473,7 +1440,7 @@
     </row>
     <row r="3" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4">
         <v>16.2</v>
@@ -1520,7 +1487,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4">
         <v>16.05</v>
@@ -1567,7 +1534,7 @@
     </row>
     <row r="5" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4">
         <v>17.18</v>
@@ -1585,7 +1552,7 @@
         <v>2.65</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="4">
         <v>1.49</v>
@@ -1606,7 +1573,7 @@
         <v>2.89</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O5" s="4">
         <v>1.22</v>
@@ -1614,7 +1581,7 @@
     </row>
     <row r="6" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4">
         <v>12.73</v>
@@ -1632,7 +1599,7 @@
         <v>0.83</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" s="4">
         <v>0.98</v>
@@ -1653,7 +1620,7 @@
         <v>0.93</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O6" s="4">
         <v>1.1599999999999999</v>
@@ -1661,7 +1628,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="4">
         <v>16.45</v>
@@ -1708,7 +1675,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>17.010000000000002</v>
@@ -1755,7 +1722,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="4">
         <v>15.6</v>
@@ -1802,7 +1769,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -1821,7 +1788,7 @@
     </row>
     <row r="11" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4">
         <v>34.86</v>
@@ -1868,7 +1835,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4">
         <v>33.729999999999997</v>
@@ -1915,7 +1882,7 @@
     </row>
     <row r="13" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
         <v>36</v>
@@ -1933,7 +1900,7 @@
         <v>6.96</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H13" s="4">
         <v>2.67</v>
@@ -1954,7 +1921,7 @@
         <v>7.79</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O13" s="4">
         <v>2.5099999999999998</v>
@@ -1962,7 +1929,7 @@
     </row>
     <row r="14" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4">
         <v>32.33</v>
@@ -1980,7 +1947,7 @@
         <v>2.69</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14" s="4">
         <v>2.33</v>
@@ -2001,7 +1968,7 @@
         <v>3.3</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O14" s="4">
         <v>2.64</v>
@@ -2009,7 +1976,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="4">
         <v>33.74</v>
@@ -2056,7 +2023,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="4">
         <v>35.78</v>
@@ -2103,7 +2070,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4">
         <v>35.549999999999997</v>
@@ -2150,7 +2117,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -2169,7 +2136,7 @@
     </row>
     <row r="19" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>27.11</v>
@@ -2216,7 +2183,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4">
         <v>22.93</v>
@@ -2263,7 +2230,7 @@
     </row>
     <row r="21" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4">
         <v>29.65</v>
@@ -2281,7 +2248,7 @@
         <v>6.8</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H21" s="4">
         <v>1.61</v>
@@ -2302,7 +2269,7 @@
         <v>7.03</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O21" s="4">
         <v>1.87</v>
@@ -2310,7 +2277,7 @@
     </row>
     <row r="22" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B22" s="4">
         <v>23.88</v>
@@ -2328,7 +2295,7 @@
         <v>2.52</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H22" s="4">
         <v>1.54</v>
@@ -2349,7 +2316,7 @@
         <v>2.59</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O22" s="4">
         <v>1.76</v>
@@ -2357,7 +2324,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="4">
         <v>25.43</v>
@@ -2404,7 +2371,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4">
         <v>25.76</v>
@@ -2451,7 +2418,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" s="4">
         <v>29.32</v>
@@ -2498,7 +2465,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -2517,7 +2484,7 @@
     </row>
     <row r="27" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B27" s="4">
         <v>1.6</v>
@@ -2564,7 +2531,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" s="4">
         <v>1.94</v>
@@ -2611,7 +2578,7 @@
     </row>
     <row r="29" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B29" s="4">
         <v>1.54</v>
@@ -2629,7 +2596,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H29" s="4">
         <v>0.06</v>
@@ -2650,7 +2617,7 @@
         <v>0.3</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O29" s="4">
         <v>0.06</v>
@@ -2658,7 +2625,7 @@
     </row>
     <row r="30" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B30" s="4">
         <v>1.32</v>
@@ -2676,7 +2643,7 @@
         <v>0.09</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H30" s="4">
         <v>7.0000000000000007E-2</v>
@@ -2697,7 +2664,7 @@
         <v>0.09</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O30" s="4">
         <v>0.04</v>
@@ -2705,7 +2672,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="4">
         <v>1.54</v>
@@ -2752,7 +2719,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" s="4">
         <v>1.67</v>
@@ -2799,7 +2766,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" s="4">
         <v>1.63</v>
@@ -2846,7 +2813,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -2865,7 +2832,7 @@
     </row>
     <row r="35" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B35" s="4">
         <v>0.94</v>
@@ -2912,7 +2879,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B36" s="4">
         <v>0.96</v>
@@ -2959,7 +2926,7 @@
     </row>
     <row r="37" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B37" s="4">
         <v>0.91</v>
@@ -2977,7 +2944,7 @@
         <v>0.04</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H37" s="4">
         <v>0.05</v>
@@ -2998,7 +2965,7 @@
         <v>0.04</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O37" s="4">
         <v>0.05</v>
@@ -3006,7 +2973,7 @@
     </row>
     <row r="38" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B38" s="4">
         <v>1.05</v>
@@ -3024,7 +2991,7 @@
         <v>0.01</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H38" s="4">
         <v>0.04</v>
@@ -3045,7 +3012,7 @@
         <v>0.01</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O38" s="4">
         <v>0.05</v>
@@ -3053,7 +3020,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" s="4">
         <v>0.95</v>
@@ -3100,7 +3067,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B40" s="4">
         <v>0.85</v>
@@ -3147,7 +3114,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B41" s="4">
         <v>0.98</v>
@@ -3194,7 +3161,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -3213,7 +3180,7 @@
     </row>
     <row r="43" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B43" s="4">
         <v>1.4</v>
@@ -3260,7 +3227,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B44" s="4">
         <v>0.9</v>
@@ -3307,7 +3274,7 @@
     </row>
     <row r="45" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B45" s="4">
         <v>1.57</v>
@@ -3325,7 +3292,7 @@
         <v>0.27</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H45" s="4">
         <v>0.08</v>
@@ -3346,7 +3313,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O45" s="4">
         <v>0.09</v>
@@ -3354,7 +3321,7 @@
     </row>
     <row r="46" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B46" s="4">
         <v>1.49</v>
@@ -3372,7 +3339,7 @@
         <v>0.1</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H46" s="4">
         <v>0.1</v>
@@ -3393,7 +3360,7 @@
         <v>0.11</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O46" s="4">
         <v>0.09</v>
@@ -3401,7 +3368,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" s="4">
         <v>1.26</v>
@@ -3448,7 +3415,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" s="4">
         <v>1.38</v>
@@ -3495,7 +3462,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49" s="4">
         <v>1.54</v>
@@ -3542,7 +3509,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -3561,7 +3528,7 @@
     </row>
     <row r="51" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B51" s="4">
         <v>0.35</v>
@@ -3608,7 +3575,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B52" s="4">
         <v>0.3</v>
@@ -3655,7 +3622,7 @@
     </row>
     <row r="53" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B53" s="4">
         <v>0.37</v>
@@ -3673,7 +3640,7 @@
         <v>0.08</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H53" s="4">
         <v>0.02</v>
@@ -3694,7 +3661,7 @@
         <v>0.08</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O53" s="4">
         <v>0.02</v>
@@ -3702,7 +3669,7 @@
     </row>
     <row r="54" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B54" s="4">
         <v>0.35</v>
@@ -3720,7 +3687,7 @@
         <v>0.02</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H54" s="4">
         <v>0.03</v>
@@ -3741,7 +3708,7 @@
         <v>0.04</v>
       </c>
       <c r="N54" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O54" s="4">
         <v>0.02</v>
@@ -3749,7 +3716,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B55" s="4">
         <v>0.33</v>
@@ -3796,7 +3763,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B56" s="4">
         <v>0.38</v>
@@ -3843,7 +3810,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B57" s="4">
         <v>0.35</v>
@@ -3890,7 +3857,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -3909,7 +3876,7 @@
     </row>
     <row r="59" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B59" s="4">
         <v>0.26</v>
@@ -3956,7 +3923,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B60" s="4">
         <v>0.2</v>
@@ -4003,7 +3970,7 @@
     </row>
     <row r="61" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B61" s="4">
         <v>0.28000000000000003</v>
@@ -4021,7 +3988,7 @@
         <v>0.06</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H61" s="4">
         <v>0.01</v>
@@ -4042,7 +4009,7 @@
         <v>0.06</v>
       </c>
       <c r="N61" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O61" s="4">
         <v>0.02</v>
@@ -4050,7 +4017,7 @@
     </row>
     <row r="62" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B62" s="4">
         <v>0.27</v>
@@ -4068,7 +4035,7 @@
         <v>0.02</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H62" s="4">
         <v>0.02</v>
@@ -4089,7 +4056,7 @@
         <v>0.02</v>
       </c>
       <c r="N62" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O62" s="4">
         <v>0.01</v>
@@ -4097,7 +4064,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B63" s="4">
         <v>0.24</v>
@@ -4144,7 +4111,7 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B64" s="4">
         <v>0.25</v>
@@ -4191,7 +4158,7 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B65" s="4">
         <v>0.28000000000000003</v>
@@ -4238,7 +4205,7 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
@@ -4257,7 +4224,7 @@
     </row>
     <row r="67" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B67" s="4">
         <v>0.09</v>
@@ -4304,7 +4271,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B68" s="4">
         <v>0.06</v>
@@ -4351,7 +4318,7 @@
     </row>
     <row r="69" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B69" s="4">
         <v>0.1</v>
@@ -4369,7 +4336,7 @@
         <v>0.01</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H69" s="4">
         <v>0.01</v>
@@ -4390,7 +4357,7 @@
         <v>0.01</v>
       </c>
       <c r="N69" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O69" s="4">
         <v>0.01</v>
@@ -4398,7 +4365,7 @@
     </row>
     <row r="70" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B70" s="4">
         <v>0.09</v>
@@ -4416,7 +4383,7 @@
         <v>0</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H70" s="4">
         <v>0</v>
@@ -4437,7 +4404,7 @@
         <v>0</v>
       </c>
       <c r="N70" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O70" s="4">
         <v>0.01</v>
@@ -4445,7 +4412,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B71" s="4">
         <v>0.08</v>
@@ -4492,7 +4459,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B72" s="4">
         <v>0.12</v>
@@ -4539,7 +4506,7 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B73" s="4">
         <v>0.1</v>
@@ -4586,7 +4553,7 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -4605,7 +4572,7 @@
     </row>
     <row r="75" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B75" s="4">
         <v>0.14000000000000001</v>
@@ -4652,7 +4619,7 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B76" s="4">
         <v>0.06</v>
@@ -4699,7 +4666,7 @@
     </row>
     <row r="77" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B77" s="4">
         <v>0.17</v>
@@ -4717,7 +4684,7 @@
         <v>0.02</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H77" s="4">
         <v>0.01</v>
@@ -4738,7 +4705,7 @@
         <v>0.02</v>
       </c>
       <c r="N77" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O77" s="4">
         <v>0.01</v>
@@ -4746,7 +4713,7 @@
     </row>
     <row r="78" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B78" s="4">
         <v>0.16</v>
@@ -4764,7 +4731,7 @@
         <v>0</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H78" s="4">
         <v>0.01</v>
@@ -4785,7 +4752,7 @@
         <v>0</v>
       </c>
       <c r="N78" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O78" s="4">
         <v>0</v>
@@ -4793,7 +4760,7 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B79" s="4">
         <v>0.12</v>
@@ -4840,7 +4807,7 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B80" s="4">
         <v>0.11</v>
@@ -4887,7 +4854,7 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B81" s="4">
         <v>0.19</v>
@@ -4934,7 +4901,7 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
@@ -4953,7 +4920,7 @@
     </row>
     <row r="83" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A83" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B83" s="4">
         <v>6.44</v>
@@ -5000,7 +4967,7 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B84" s="4">
         <v>6.75</v>
@@ -5047,7 +5014,7 @@
     </row>
     <row r="85" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B85" s="4">
         <v>6.57</v>
@@ -5065,7 +5032,7 @@
         <v>1.41</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H85" s="4">
         <v>0.39</v>
@@ -5086,7 +5053,7 @@
         <v>1.55</v>
       </c>
       <c r="N85" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O85" s="4">
         <v>0.4</v>
@@ -5094,7 +5061,7 @@
     </row>
     <row r="86" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B86" s="4">
         <v>5.48</v>
@@ -5112,7 +5079,7 @@
         <v>0.52</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H86" s="4">
         <v>0.34</v>
@@ -5133,7 +5100,7 @@
         <v>0.59</v>
       </c>
       <c r="N86" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O86" s="4">
         <v>0.33</v>
@@ -5141,7 +5108,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B87" s="4">
         <v>6.5</v>
@@ -5188,7 +5155,7 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B88" s="4">
         <v>6.29</v>
@@ -5235,7 +5202,7 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B89" s="4">
         <v>6.45</v>
@@ -5282,7 +5249,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -5301,7 +5268,7 @@
     </row>
     <row r="91" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A91" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B91" s="4">
         <v>5.53</v>
@@ -5348,7 +5315,7 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B92" s="4">
         <v>5.88</v>
@@ -5395,7 +5362,7 @@
     </row>
     <row r="93" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B93" s="4">
         <v>5.68</v>
@@ -5413,7 +5380,7 @@
         <v>1.35</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H93" s="4">
         <v>0.34</v>
@@ -5434,7 +5401,7 @@
         <v>1.5</v>
       </c>
       <c r="N93" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O93" s="4">
         <v>0.37</v>
@@ -5442,7 +5409,7 @@
     </row>
     <row r="94" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B94" s="4">
         <v>4.41</v>
@@ -5460,7 +5427,7 @@
         <v>0.5</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H94" s="4">
         <v>0.31</v>
@@ -5481,7 +5448,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="N94" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O94" s="4">
         <v>0.31</v>
@@ -5489,7 +5456,7 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B95" s="4">
         <v>5.69</v>
@@ -5536,7 +5503,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B96" s="4">
         <v>5.36</v>
@@ -5583,7 +5550,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B97" s="4">
         <v>5.44</v>
@@ -5630,7 +5597,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="21"/>
@@ -5649,7 +5616,7 @@
     </row>
     <row r="99" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A99" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B99" s="4">
         <v>0.91</v>
@@ -5696,7 +5663,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B100" s="4">
         <v>0.87</v>
@@ -5743,7 +5710,7 @@
     </row>
     <row r="101" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B101" s="4">
         <v>0.89</v>
@@ -5761,7 +5728,7 @@
         <v>0.06</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H101" s="4">
         <v>0.04</v>
@@ -5782,7 +5749,7 @@
         <v>0.05</v>
       </c>
       <c r="N101" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O101" s="4">
         <v>0.02</v>
@@ -5790,7 +5757,7 @@
     </row>
     <row r="102" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B102" s="4">
         <v>1.07</v>
@@ -5808,7 +5775,7 @@
         <v>0.02</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H102" s="4">
         <v>0.03</v>
@@ -5829,7 +5796,7 @@
         <v>0.01</v>
       </c>
       <c r="N102" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O102" s="4">
         <v>0.02</v>
@@ -5837,7 +5804,7 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B103" s="4">
         <v>0.81</v>
@@ -5884,7 +5851,7 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B104" s="4">
         <v>0.94</v>
@@ -5931,7 +5898,7 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B105" s="4">
         <v>1.01</v>
@@ -5978,7 +5945,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="21"/>
@@ -5997,7 +5964,7 @@
     </row>
     <row r="107" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A107" s="20" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B107" s="4">
         <v>5.8</v>
@@ -6044,7 +6011,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B108" s="4">
         <v>4.1500000000000004</v>
@@ -6091,7 +6058,7 @@
     </row>
     <row r="109" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B109" s="4">
         <v>6.6</v>
@@ -6109,7 +6076,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H109" s="4">
         <v>0.38</v>
@@ -6130,7 +6097,7 @@
         <v>1.18</v>
       </c>
       <c r="N109" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O109" s="4">
         <v>0.38</v>
@@ -6138,7 +6105,7 @@
     </row>
     <row r="110" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B110" s="4">
         <v>5.26</v>
@@ -6156,7 +6123,7 @@
         <v>0.45</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H110" s="4">
         <v>0.32</v>
@@ -6177,7 +6144,7 @@
         <v>0.48</v>
       </c>
       <c r="N110" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O110" s="4">
         <v>0.37</v>
@@ -6185,7 +6152,7 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B111" s="4">
         <v>5.4</v>
@@ -6232,7 +6199,7 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B112" s="4">
         <v>5.67</v>
@@ -6279,7 +6246,7 @@
     </row>
     <row r="113" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B113" s="4">
         <v>6.23</v>
@@ -6326,7 +6293,7 @@
     </row>
     <row r="114" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A114" s="28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -6338,7 +6305,7 @@
     </row>
     <row r="115" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A115" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
@@ -6350,12 +6317,12 @@
     </row>
     <row r="116" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B117" s="10"/>
       <c r="C117" s="10"/>

</xml_diff>

<commit_message>
changes the excell files
</commit_message>
<xml_diff>
--- a/data/Food_nutrition_Intake/food_table1.xlsx
+++ b/data/Food_nutrition_Intake/food_table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20201077\Desktop\DorukGüngör\Eindhoven\Data_Science_AI\Knowledge_Engineering\Knowledge-Engineering-2AMD20-\data\Food_nutrition_Intake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778AFB5F-71A8-4A67-BC6F-935A6968AF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB380F3F-7E75-4E88-8356-98B7B2430F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,21 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="31">
   <si>
     <t>Food group</t>
-  </si>
-  <si>
-    <t>Added sugar (tsp)</t>
   </si>
   <si>
     <t>Discretionary oils (g)</t>
   </si>
   <si>
     <t>Dairy (cup)</t>
-  </si>
-  <si>
-    <t>Fruit (cup)</t>
   </si>
   <si>
     <t>Vegetables: total (cup)</t>
@@ -66,9 +60,6 @@
   </si>
   <si>
     <t>Vegetables: red and orange without tomatoes (cup)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Children age 2–19</t>
   </si>
   <si>
     <r>
@@ -144,12 +135,6 @@
     <t xml:space="preserve">   Total population</t>
   </si>
   <si>
-    <t xml:space="preserve">      Adults age 20–64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Adults age 20–6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total </t>
   </si>
   <si>
@@ -172,6 +157,18 @@
   </si>
   <si>
     <t xml:space="preserve">Other </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Adults</t>
+  </si>
+  <si>
+    <t>Fruits (cup)</t>
+  </si>
+  <si>
+    <t>Added sugars (tsp)</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1320,30 +1317,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -1355,7 +1352,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>16.2</v>
@@ -1381,7 +1378,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4">
         <v>16.05</v>
@@ -1407,7 +1404,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4">
         <v>17.18</v>
@@ -1425,7 +1422,7 @@
         <v>2.65</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4">
         <v>1.49</v>
@@ -1433,7 +1430,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -1445,7 +1442,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>34.86</v>
@@ -1471,7 +1468,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4">
         <v>33.729999999999997</v>
@@ -1497,7 +1494,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4">
         <v>36</v>
@@ -1515,7 +1512,7 @@
         <v>6.96</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H9" s="4">
         <v>2.67</v>
@@ -1523,7 +1520,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1535,7 +1532,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
         <v>27.11</v>
@@ -1561,7 +1558,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4">
         <v>22.93</v>
@@ -1587,7 +1584,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4">
         <v>29.65</v>
@@ -1605,7 +1602,7 @@
         <v>6.8</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H13" s="4">
         <v>1.61</v>
@@ -1613,7 +1610,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -1625,7 +1622,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>1.6</v>
@@ -1651,7 +1648,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4">
         <v>1.94</v>
@@ -1677,7 +1674,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4">
         <v>1.54</v>
@@ -1695,7 +1692,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4">
         <v>0.06</v>
@@ -1703,7 +1700,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1715,7 +1712,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
         <v>0.94</v>
@@ -1741,7 +1738,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4">
         <v>0.96</v>
@@ -1767,7 +1764,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4">
         <v>0.91</v>
@@ -1785,7 +1782,7 @@
         <v>0.04</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H21" s="4">
         <v>0.05</v>
@@ -1793,7 +1790,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -1805,7 +1802,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4">
         <v>1.4</v>
@@ -1831,7 +1828,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B24" s="4">
         <v>0.9</v>
@@ -1857,7 +1854,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B25" s="4">
         <v>1.57</v>
@@ -1875,7 +1872,7 @@
         <v>0.27</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H25" s="4">
         <v>0.08</v>
@@ -1883,7 +1880,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -1895,7 +1892,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B27" s="4">
         <v>0.35</v>
@@ -1921,7 +1918,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4">
         <v>0.3</v>
@@ -1947,7 +1944,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4">
         <v>0.37</v>
@@ -1965,7 +1962,7 @@
         <v>0.08</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H29" s="4">
         <v>0.02</v>
@@ -1973,7 +1970,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1985,7 +1982,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B31" s="4">
         <v>0.26</v>
@@ -2011,7 +2008,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4">
         <v>0.2</v>
@@ -2037,7 +2034,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4">
         <v>0.28000000000000003</v>
@@ -2055,7 +2052,7 @@
         <v>0.06</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H33" s="4">
         <v>0.01</v>
@@ -2063,7 +2060,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -2075,7 +2072,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B35" s="4">
         <v>0.09</v>
@@ -2101,7 +2098,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B36" s="4">
         <v>0.06</v>
@@ -2127,7 +2124,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B37" s="4">
         <v>0.1</v>
@@ -2145,7 +2142,7 @@
         <v>0.01</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H37" s="4">
         <v>0.01</v>
@@ -2153,7 +2150,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
@@ -2165,7 +2162,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B39" s="4">
         <v>0.14000000000000001</v>
@@ -2191,7 +2188,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B40" s="4">
         <v>0.06</v>
@@ -2217,7 +2214,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B41" s="4">
         <v>0.17</v>
@@ -2235,7 +2232,7 @@
         <v>0.02</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H41" s="4">
         <v>0.01</v>
@@ -2243,7 +2240,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B43" s="4">
         <v>6.44</v>
@@ -2281,7 +2278,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B44" s="4">
         <v>6.75</v>
@@ -2307,7 +2304,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B45" s="4">
         <v>6.57</v>
@@ -2325,7 +2322,7 @@
         <v>1.41</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H45" s="4">
         <v>0.39</v>
@@ -2333,7 +2330,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
@@ -2345,7 +2342,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B47" s="4">
         <v>5.53</v>
@@ -2371,7 +2368,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B48" s="4">
         <v>5.88</v>
@@ -2397,7 +2394,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B49" s="4">
         <v>5.68</v>
@@ -2415,7 +2412,7 @@
         <v>1.35</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H49" s="4">
         <v>0.34</v>
@@ -2423,7 +2420,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
@@ -2435,7 +2432,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B51" s="4">
         <v>0.91</v>
@@ -2461,7 +2458,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B52" s="4">
         <v>0.87</v>
@@ -2487,7 +2484,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B53" s="4">
         <v>0.89</v>
@@ -2505,7 +2502,7 @@
         <v>0.06</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H53" s="4">
         <v>0.04</v>
@@ -2513,7 +2510,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
@@ -2525,7 +2522,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B55" s="4">
         <v>5.8</v>
@@ -2551,7 +2548,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B56" s="4">
         <v>4.1500000000000004</v>
@@ -2577,7 +2574,7 @@
     </row>
     <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B57" s="4">
         <v>6.6</v>
@@ -2595,7 +2592,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H57" s="4">
         <v>0.38</v>
@@ -2603,7 +2600,7 @@
     </row>
     <row r="58" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A58" s="26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2615,7 +2612,7 @@
     </row>
     <row r="59" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
@@ -2627,12 +2624,12 @@
     </row>
     <row r="60" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A60" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -2700,15 +2697,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22EB0B92-AB8A-4071-B154-D4529DC67D11}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.109375" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
@@ -2723,30 +2720,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2758,7 +2755,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>16.940000000000001</v>
@@ -2784,7 +2781,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4">
         <v>16.55</v>
@@ -2810,7 +2807,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4">
         <v>17.760000000000002</v>
@@ -2828,7 +2825,7 @@
         <v>2.89</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4">
         <v>1.22</v>
@@ -2836,7 +2833,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2848,7 +2845,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>36.24</v>
@@ -2874,7 +2871,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4">
         <v>33.840000000000003</v>
@@ -2900,7 +2897,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4">
         <v>37.32</v>
@@ -2918,7 +2915,7 @@
         <v>7.79</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H9" s="4">
         <v>2.5099999999999998</v>
@@ -2926,7 +2923,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2938,7 +2935,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
         <v>29.12</v>
@@ -2964,7 +2961,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4">
         <v>24.68</v>
@@ -2990,7 +2987,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4">
         <v>31.36</v>
@@ -3008,7 +3005,7 @@
         <v>7.03</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H13" s="4">
         <v>1.87</v>
@@ -3016,7 +3013,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -3028,7 +3025,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>1.53</v>
@@ -3054,7 +3051,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4">
         <v>1.81</v>
@@ -3080,7 +3077,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4">
         <v>1.47</v>
@@ -3098,7 +3095,7 @@
         <v>0.3</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4">
         <v>0.06</v>
@@ -3106,7 +3103,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3118,7 +3115,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
         <v>0.93</v>
@@ -3144,7 +3141,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4">
         <v>1.1000000000000001</v>
@@ -3170,7 +3167,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4">
         <v>0.83</v>
@@ -3188,7 +3185,7 @@
         <v>0.04</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H21" s="4">
         <v>0.05</v>
@@ -3196,7 +3193,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3208,7 +3205,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4">
         <v>1.39</v>
@@ -3234,7 +3231,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B24" s="4">
         <v>0.86</v>
@@ -3260,7 +3257,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B25" s="4">
         <v>1.56</v>
@@ -3278,7 +3275,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H25" s="4">
         <v>0.09</v>
@@ -3286,7 +3283,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3298,7 +3295,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B27" s="4">
         <v>0.36</v>
@@ -3324,7 +3321,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4">
         <v>0.28999999999999998</v>
@@ -3350,7 +3347,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4">
         <v>0.38</v>
@@ -3368,7 +3365,7 @@
         <v>0.08</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H29" s="4">
         <v>0.02</v>
@@ -3376,7 +3373,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3388,7 +3385,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B31" s="4">
         <v>0.26</v>
@@ -3414,7 +3411,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4">
         <v>0.19</v>
@@ -3440,7 +3437,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4">
         <v>0.28000000000000003</v>
@@ -3458,7 +3455,7 @@
         <v>0.06</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H33" s="4">
         <v>0.02</v>
@@ -3466,7 +3463,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -3478,7 +3475,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B35" s="4">
         <v>0.09</v>
@@ -3504,7 +3501,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B36" s="4">
         <v>0.06</v>
@@ -3530,7 +3527,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B37" s="4">
         <v>0.1</v>
@@ -3548,7 +3545,7 @@
         <v>0.01</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H37" s="4">
         <v>0.01</v>
@@ -3556,7 +3553,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -3568,7 +3565,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B39" s="4">
         <v>0.14000000000000001</v>
@@ -3594,7 +3591,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B40" s="4">
         <v>0.06</v>
@@ -3620,7 +3617,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B41" s="4">
         <v>0.17</v>
@@ -3638,7 +3635,7 @@
         <v>0.02</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H41" s="4">
         <v>0.01</v>
@@ -3646,7 +3643,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -3658,7 +3655,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B43" s="4">
         <v>6.64</v>
@@ -3684,7 +3681,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B44" s="4">
         <v>6.75</v>
@@ -3710,7 +3707,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B45" s="4">
         <v>6.81</v>
@@ -3728,7 +3725,7 @@
         <v>1.55</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H45" s="4">
         <v>0.4</v>
@@ -3736,7 +3733,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3748,7 +3745,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B47" s="4">
         <v>5.79</v>
@@ -3774,7 +3771,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B48" s="4">
         <v>5.9</v>
@@ -3800,7 +3797,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B49" s="4">
         <v>6.03</v>
@@ -3818,7 +3815,7 @@
         <v>1.5</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H49" s="4">
         <v>0.37</v>
@@ -3826,7 +3823,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -3838,7 +3835,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B51" s="4">
         <v>0.84</v>
@@ -3864,7 +3861,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B52" s="4">
         <v>0.85</v>
@@ -3890,7 +3887,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B53" s="4">
         <v>0.78</v>
@@ -3908,7 +3905,7 @@
         <v>0.05</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H53" s="4">
         <v>0.02</v>
@@ -3916,7 +3913,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3928,7 +3925,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B55" s="4">
         <v>5.84</v>
@@ -3954,7 +3951,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B56" s="4">
         <v>4.28</v>
@@ -3978,9 +3975,9 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B57" s="4">
         <v>6.46</v>
@@ -3998,11 +3995,46 @@
         <v>1.18</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H57" s="4">
         <v>0.38</v>
       </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="11"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="8"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="11"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="8"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>